<commit_message>
Updated Supervisor, FYP Coordinator Class
</commit_message>
<xml_diff>
--- a/App/data/faculty_list.xlsx
+++ b/App/data/faculty_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Coding\Coding Projects\Github Repo\OOP-FYP-Management-Project\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A89B9C-8DEF-4941-8693-AD8CDF32F5A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C7C9FE-82F1-4309-91A0-5524A64B5936}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="229">
   <si>
     <t>Name</t>
   </si>
@@ -713,6 +713,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>num_assigned</t>
   </si>
 </sst>
 </file>
@@ -1138,12 +1141,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1153,7 +1156,7 @@
     <col min="3" max="3" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>227</v>
       </c>
@@ -1163,8 +1166,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>156</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>158</v>
       </c>
@@ -1241,7 +1247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>159</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>160</v>
       </c>
@@ -1263,7 +1269,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>161</v>
       </c>
@@ -1274,7 +1280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -1285,7 +1291,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>163</v>
       </c>
@@ -1296,7 +1302,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -1307,7 +1313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Major Update to OOP Structure, Pending Requests
</commit_message>
<xml_diff>
--- a/App/data/faculty_list.xlsx
+++ b/App/data/faculty_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugen\Desktop\Coding\Coding Projects\Github Repo\OOP-FYP-Management-Project\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C7C9FE-82F1-4309-91A0-5524A64B5936}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68A6699-F76D-42EB-9F50-723D1AEADC5F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView xWindow="3732" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
   <sheets>
     <sheet name="30Aug2022_FYP Examiner List" sheetId="1" r:id="rId1"/>
@@ -1146,7 +1146,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D76" sqref="D2:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,6 +1180,9 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1191,6 +1194,9 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1202,6 +1208,9 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1213,6 +1222,9 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1224,6 +1236,9 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1235,6 +1250,9 @@
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1246,6 +1264,9 @@
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1257,6 +1278,9 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1268,6 +1292,9 @@
       <c r="C10" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1279,6 +1306,9 @@
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1290,6 +1320,9 @@
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1301,6 +1334,9 @@
       <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1312,6 +1348,9 @@
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1323,6 +1362,9 @@
       <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1334,8 +1376,11 @@
       <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -1345,8 +1390,11 @@
       <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -1356,8 +1404,11 @@
       <c r="C18" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -1367,8 +1418,11 @@
       <c r="C19" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>170</v>
       </c>
@@ -1378,8 +1432,11 @@
       <c r="C20" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -1389,8 +1446,11 @@
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>172</v>
       </c>
@@ -1400,8 +1460,11 @@
       <c r="C22" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>173</v>
       </c>
@@ -1411,8 +1474,11 @@
       <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>174</v>
       </c>
@@ -1422,8 +1488,11 @@
       <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>175</v>
       </c>
@@ -1433,8 +1502,11 @@
       <c r="C25" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -1444,8 +1516,11 @@
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>177</v>
       </c>
@@ -1455,8 +1530,11 @@
       <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -1466,8 +1544,11 @@
       <c r="C28" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>179</v>
       </c>
@@ -1477,8 +1558,11 @@
       <c r="C29" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>180</v>
       </c>
@@ -1488,8 +1572,11 @@
       <c r="C30" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>181</v>
       </c>
@@ -1499,8 +1586,11 @@
       <c r="C31" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -1510,8 +1600,11 @@
       <c r="C32" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -1521,8 +1614,11 @@
       <c r="C33" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -1532,8 +1628,11 @@
       <c r="C34" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>185</v>
       </c>
@@ -1543,8 +1642,11 @@
       <c r="C35" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>186</v>
       </c>
@@ -1554,8 +1656,11 @@
       <c r="C36" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>187</v>
       </c>
@@ -1565,8 +1670,11 @@
       <c r="C37" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -1576,8 +1684,11 @@
       <c r="C38" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>189</v>
       </c>
@@ -1587,8 +1698,11 @@
       <c r="C39" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -1598,8 +1712,11 @@
       <c r="C40" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>191</v>
       </c>
@@ -1609,8 +1726,11 @@
       <c r="C41" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -1620,8 +1740,11 @@
       <c r="C42" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -1631,8 +1754,11 @@
       <c r="C43" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>194</v>
       </c>
@@ -1642,8 +1768,11 @@
       <c r="C44" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>195</v>
       </c>
@@ -1653,8 +1782,11 @@
       <c r="C45" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>196</v>
       </c>
@@ -1664,8 +1796,11 @@
       <c r="C46" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>197</v>
       </c>
@@ -1675,8 +1810,11 @@
       <c r="C47" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>198</v>
       </c>
@@ -1686,8 +1824,11 @@
       <c r="C48" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>199</v>
       </c>
@@ -1697,8 +1838,11 @@
       <c r="C49" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>200</v>
       </c>
@@ -1708,8 +1852,11 @@
       <c r="C50" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -1719,8 +1866,11 @@
       <c r="C51" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>202</v>
       </c>
@@ -1730,8 +1880,11 @@
       <c r="C52" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>203</v>
       </c>
@@ -1741,8 +1894,11 @@
       <c r="C53" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>204</v>
       </c>
@@ -1752,8 +1908,11 @@
       <c r="C54" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>205</v>
       </c>
@@ -1763,8 +1922,11 @@
       <c r="C55" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>206</v>
       </c>
@@ -1774,8 +1936,11 @@
       <c r="C56" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>207</v>
       </c>
@@ -1785,8 +1950,11 @@
       <c r="C57" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>208</v>
       </c>
@@ -1796,8 +1964,11 @@
       <c r="C58" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>209</v>
       </c>
@@ -1807,8 +1978,11 @@
       <c r="C59" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>210</v>
       </c>
@@ -1818,8 +1992,11 @@
       <c r="C60" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>211</v>
       </c>
@@ -1829,8 +2006,11 @@
       <c r="C61" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>212</v>
       </c>
@@ -1840,8 +2020,11 @@
       <c r="C62" s="13" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>213</v>
       </c>
@@ -1851,8 +2034,11 @@
       <c r="C63" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>214</v>
       </c>
@@ -1862,8 +2048,11 @@
       <c r="C64" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -1873,8 +2062,11 @@
       <c r="C65" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>216</v>
       </c>
@@ -1884,8 +2076,11 @@
       <c r="C66" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>217</v>
       </c>
@@ -1895,8 +2090,11 @@
       <c r="C67" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>218</v>
       </c>
@@ -1906,8 +2104,11 @@
       <c r="C68" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>219</v>
       </c>
@@ -1917,8 +2118,11 @@
       <c r="C69" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>220</v>
       </c>
@@ -1928,8 +2132,11 @@
       <c r="C70" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>221</v>
       </c>
@@ -1939,8 +2146,11 @@
       <c r="C71" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>222</v>
       </c>
@@ -1950,8 +2160,11 @@
       <c r="C72" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>223</v>
       </c>
@@ -1961,8 +2174,11 @@
       <c r="C73" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>224</v>
       </c>
@@ -1972,8 +2188,11 @@
       <c r="C74" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>225</v>
       </c>
@@ -1983,8 +2202,11 @@
       <c r="C75" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>226</v>
       </c>
@@ -1994,11 +2216,14 @@
       <c r="C76" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B79" s="4"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B80" s="4"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
registered proj to student
</commit_message>
<xml_diff>
--- a/App/data/faculty_list.xlsx
+++ b/App/data/faculty_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liekzhewong/Desktop/Desktop - Liek’s MacBook Pro/SC2002/OOP-FYP-Management-Project/App/data/"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="229">
   <si>
     <t>Name</t>
   </si>
@@ -722,6 +722,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1117,9 +1118,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="22" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="25.5"/>
+    <col min="2" max="2" customWidth="true" style="4" width="22.0"/>
+    <col min="3" max="3" customWidth="true" width="25.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1137,1053 +1138,1053 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>152</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>153</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>0</v>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>154</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s" s="4">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>155</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="D5" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>156</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D6">
-        <v>0</v>
+      <c r="D6" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>157</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D7">
-        <v>0</v>
+      <c r="D7" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>158</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D8">
-        <v>0</v>
+      <c r="D8" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>159</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D9">
-        <v>0</v>
+      <c r="D9" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>160</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s" s="4">
         <v>129</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="D10">
-        <v>0</v>
+      <c r="D10" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>161</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D11">
-        <v>0</v>
+      <c r="D11" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>162</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D12">
-        <v>0</v>
+      <c r="D12" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>163</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D13">
-        <v>0</v>
+      <c r="D13" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>164</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s" s="4">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="D14" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>165</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s" s="4">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="D15" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>166</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s" s="4">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="D16">
-        <v>0</v>
+      <c r="D16" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>167</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s" s="4">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="D17">
-        <v>0</v>
+      <c r="D17" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>168</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s" s="4">
         <v>32</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="D18">
-        <v>0</v>
+      <c r="D18" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>169</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s" s="4">
         <v>146</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>147</v>
       </c>
-      <c r="D19">
-        <v>0</v>
+      <c r="D19" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>170</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s" s="4">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D20">
-        <v>0</v>
+      <c r="D20" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>171</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s" s="4">
         <v>36</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="D21">
-        <v>0</v>
+      <c r="D21" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>172</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s" s="4">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="D22">
-        <v>0</v>
+      <c r="D22" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>173</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s" s="4">
         <v>40</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="D23">
-        <v>0</v>
+      <c r="D23" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>174</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s" s="4">
         <v>42</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="D24">
-        <v>0</v>
+      <c r="D24" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>175</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s" s="4">
         <v>44</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="D25">
-        <v>0</v>
+      <c r="D25" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>176</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s" s="4">
         <v>46</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="D26">
-        <v>0</v>
+      <c r="D26" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>177</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s" s="4">
         <v>48</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="D27">
-        <v>0</v>
+      <c r="D27" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>178</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s" s="4">
         <v>136</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" t="s" s="0">
         <v>137</v>
       </c>
-      <c r="D28">
-        <v>0</v>
+      <c r="D28" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>179</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s" s="4">
         <v>50</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="D29">
-        <v>0</v>
+      <c r="D29" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>180</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" t="s" s="4">
         <v>130</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="D30">
-        <v>0</v>
+      <c r="D30" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>181</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s" s="4">
         <v>52</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="D31">
-        <v>0</v>
+      <c r="D31" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>182</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" t="s" s="4">
         <v>126</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" t="s" s="0">
         <v>133</v>
       </c>
-      <c r="D32">
-        <v>0</v>
+      <c r="D32" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>183</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" t="s" s="4">
         <v>54</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="D33">
-        <v>0</v>
+      <c r="D33" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" t="s" s="0">
         <v>184</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" t="s" s="4">
         <v>56</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="D34">
-        <v>0</v>
+      <c r="D34" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" t="s" s="0">
         <v>185</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" t="s" s="4">
         <v>58</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="D35">
-        <v>0</v>
+      <c r="D35" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" t="s" s="0">
         <v>186</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s" s="4">
         <v>60</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="D36">
-        <v>0</v>
+      <c r="D36" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" t="s" s="0">
         <v>187</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" t="s" s="4">
         <v>62</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="D37">
-        <v>0</v>
+      <c r="D37" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" t="s" s="0">
         <v>188</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" t="s" s="4">
         <v>64</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="D38">
-        <v>0</v>
+      <c r="D38" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" t="s" s="0">
         <v>189</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" t="s" s="4">
         <v>66</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="D39">
-        <v>0</v>
+      <c r="D39" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" t="s" s="0">
         <v>190</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" t="s" s="4">
         <v>68</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="D40">
-        <v>0</v>
+      <c r="D40" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" t="s" s="0">
         <v>191</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" t="s" s="4">
         <v>127</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" t="s" s="0">
         <v>134</v>
       </c>
-      <c r="D41">
-        <v>0</v>
+      <c r="D41" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" t="s" s="0">
         <v>192</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" t="s" s="4">
         <v>128</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="D42">
-        <v>0</v>
+      <c r="D42" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" t="s" s="0">
         <v>193</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" t="s" s="4">
         <v>70</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="D43">
-        <v>0</v>
+      <c r="D43" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" t="s" s="0">
         <v>194</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="D44">
-        <v>0</v>
+      <c r="D44" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="A45" t="s" s="0">
         <v>195</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="D45">
-        <v>0</v>
+      <c r="D45" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" t="s" s="0">
         <v>196</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" t="s" s="4">
         <v>76</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="D46">
-        <v>0</v>
+      <c r="D46" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" t="s" s="0">
         <v>197</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" t="s" s="4">
         <v>138</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" t="s" s="0">
         <v>139</v>
       </c>
-      <c r="D47">
-        <v>0</v>
+      <c r="D47" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" t="s" s="4">
         <v>78</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="D48">
-        <v>0</v>
+      <c r="D48" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A49" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" t="s" s="4">
         <v>80</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="D49">
-        <v>0</v>
+      <c r="D49" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="A50" t="s" s="0">
         <v>200</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" t="s" s="4">
         <v>82</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="D50">
-        <v>0</v>
+      <c r="D50" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="A51" t="s" s="0">
         <v>201</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" t="s" s="4">
         <v>150</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" t="s" s="0">
         <v>151</v>
       </c>
-      <c r="D51">
-        <v>0</v>
+      <c r="D51" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="A52" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" t="s" s="4">
         <v>84</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="D52">
-        <v>0</v>
+      <c r="D52" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="A53" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" t="s" s="4">
         <v>86</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="D53">
-        <v>0</v>
+      <c r="D53" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="A54" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" t="s" s="4">
         <v>88</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="D54">
-        <v>0</v>
+      <c r="D54" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="A55" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" t="s" s="4">
         <v>90</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="D55">
-        <v>0</v>
+      <c r="D55" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" t="s" s="0">
         <v>206</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" t="s" s="4">
         <v>92</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="D56">
-        <v>0</v>
+      <c r="D56" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" t="s" s="0">
         <v>207</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" t="s" s="4">
         <v>94</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="D57">
-        <v>0</v>
+      <c r="D57" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" t="s" s="4">
         <v>96</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="D58">
-        <v>0</v>
+      <c r="D58" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="A59" t="s" s="0">
         <v>209</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" t="s" s="4">
         <v>98</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="D59">
-        <v>0</v>
+      <c r="D59" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" t="s" s="0">
         <v>210</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" t="s" s="4">
         <v>100</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="D60">
-        <v>0</v>
+      <c r="D60" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" t="s" s="0">
         <v>211</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" t="s" s="4">
         <v>102</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="D61">
-        <v>0</v>
+      <c r="D61" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" t="s" s="0">
         <v>212</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" t="s" s="4">
         <v>148</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" t="s" s="0">
         <v>149</v>
       </c>
-      <c r="D62">
-        <v>0</v>
+      <c r="D62" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" t="s" s="0">
         <v>213</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" t="s" s="4">
         <v>104</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="D63">
-        <v>0</v>
+      <c r="D63" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="A64" t="s" s="0">
         <v>214</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" t="s" s="4">
         <v>106</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="D64">
-        <v>0</v>
+      <c r="D64" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="A65" t="s" s="0">
         <v>215</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" t="s" s="4">
         <v>108</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="D65">
-        <v>0</v>
+      <c r="D65" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="A66" t="s" s="0">
         <v>216</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" t="s" s="4">
         <v>140</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" t="s" s="0">
         <v>143</v>
       </c>
-      <c r="D66">
-        <v>0</v>
+      <c r="D66" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="A67" t="s" s="0">
         <v>217</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" t="s" s="4">
         <v>141</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" t="s" s="0">
         <v>144</v>
       </c>
-      <c r="D67">
-        <v>0</v>
+      <c r="D67" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="A68" t="s" s="0">
         <v>218</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" t="s" s="4">
         <v>110</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="D68">
-        <v>0</v>
+      <c r="D68" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="A69" t="s" s="0">
         <v>219</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" t="s" s="4">
         <v>142</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" t="s" s="0">
         <v>145</v>
       </c>
-      <c r="D69">
-        <v>0</v>
+      <c r="D69" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="A70" t="s" s="0">
         <v>220</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" t="s" s="4">
         <v>112</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="D70">
-        <v>0</v>
+      <c r="D70" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="A71" t="s" s="0">
         <v>221</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" t="s" s="4">
         <v>114</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="D71">
-        <v>0</v>
+      <c r="D71" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="A72" t="s" s="0">
         <v>222</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" t="s" s="4">
         <v>116</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="D72">
-        <v>0</v>
+      <c r="D72" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="A73" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" t="s" s="4">
         <v>118</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="D73">
-        <v>0</v>
+      <c r="D73" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="A74" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" t="s" s="4">
         <v>120</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="D74">
-        <v>0</v>
+      <c r="D74" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="A75" t="s" s="0">
         <v>225</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" t="s" s="4">
         <v>122</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="D75">
-        <v>0</v>
+      <c r="D75" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="A76" t="s" s="0">
         <v>226</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" t="s" s="4">
         <v>124</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="D76">
-        <v>0</v>
+      <c r="D76" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Restructured Request, Changed Student
</commit_message>
<xml_diff>
--- a/App/data/faculty_list.xlsx
+++ b/App/data/faculty_list.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="229">
   <si>
     <t>Name</t>
   </si>
@@ -1148,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>